<commit_message>
N.Phuong chỉnh sửa 10:48 21-02
</commit_message>
<xml_diff>
--- a/MAP.xlsx
+++ b/MAP.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Deadline\CTDLnGT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{851F32BB-A458-450A-8C49-0D848E098FB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B3DA2AE-5BF9-409D-AF36-3F6D516864CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{41A466AB-4909-4B18-947B-88C6910C9A97}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{41A466AB-4909-4B18-947B-88C6910C9A97}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="LIBS" sheetId="1" r:id="rId1"/>
+    <sheet name="VAR_MAP" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>MAIN</t>
   </si>
@@ -69,6 +70,24 @@
   </si>
   <si>
     <t>hanh_khach</t>
+  </si>
+  <si>
+    <t>MayBay</t>
+  </si>
+  <si>
+    <t>SoHieu</t>
+  </si>
+  <si>
+    <t>KieuDang</t>
+  </si>
+  <si>
+    <t>SoCot</t>
+  </si>
+  <si>
+    <t>SoDong</t>
+  </si>
+  <si>
+    <t>ChuyenBay</t>
   </si>
 </sst>
 </file>
@@ -547,7 +566,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B27D530B-6906-4022-8FAA-0D0EFC2012E3}">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -694,4 +713,50 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A38A2D5-255B-4875-B229-79E683E1EA85}">
+  <dimension ref="B3:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="18.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add map, .ignore, maybay.h
</commit_message>
<xml_diff>
--- a/MAP.xlsx
+++ b/MAP.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Deadline\CTDLnGT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CTDLnGT\CTDL-GT_N7_D21CQCN02-N\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B3DA2AE-5BF9-409D-AF36-3F6D516864CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B06440-C5C3-4A2F-A345-AC78A4CF9F29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{41A466AB-4909-4B18-947B-88C6910C9A97}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{41A466AB-4909-4B18-947B-88C6910C9A97}"/>
   </bookViews>
   <sheets>
-    <sheet name="LIBS" sheetId="1" r:id="rId1"/>
-    <sheet name="VAR_MAP" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,9 +27,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="42">
   <si>
     <t>MAIN</t>
   </si>
@@ -72,29 +69,104 @@
     <t>hanh_khach</t>
   </si>
   <si>
-    <t>MayBay</t>
-  </si>
-  <si>
-    <t>SoHieu</t>
-  </si>
-  <si>
-    <t>KieuDang</t>
-  </si>
-  <si>
-    <t>SoCot</t>
-  </si>
-  <si>
-    <t>SoDong</t>
-  </si>
-  <si>
-    <t>ChuyenBay</t>
+    <t>MAYBAY</t>
+  </si>
+  <si>
+    <t>SOHIEUMB</t>
+  </si>
+  <si>
+    <t>LOAIMB</t>
+  </si>
+  <si>
+    <t>SODAY</t>
+  </si>
+  <si>
+    <t>SODONG</t>
+  </si>
+  <si>
+    <t>CHAR15</t>
+  </si>
+  <si>
+    <t>CHAR40</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>CHUYENBAY</t>
+  </si>
+  <si>
+    <t>MACB</t>
+  </si>
+  <si>
+    <t>NOIDEN</t>
+  </si>
+  <si>
+    <t>TRANGTHAI</t>
+  </si>
+  <si>
+    <t>DSVE</t>
+  </si>
+  <si>
+    <t>NGAYGIO</t>
+  </si>
+  <si>
+    <t>STRING</t>
+  </si>
+  <si>
+    <t>CLASS</t>
+  </si>
+  <si>
+    <t>STRUCT</t>
+  </si>
+  <si>
+    <t>IDVE</t>
+  </si>
+  <si>
+    <t>CMND</t>
+  </si>
+  <si>
+    <t>NGAY</t>
+  </si>
+  <si>
+    <t>THANG</t>
+  </si>
+  <si>
+    <t>NAM</t>
+  </si>
+  <si>
+    <t>GIO</t>
+  </si>
+  <si>
+    <t>PHUT</t>
+  </si>
+  <si>
+    <t>NOTE: MẢNG CON TRỎ TỐI ĐA 300 MÁY BAY</t>
+  </si>
+  <si>
+    <t>HANHKHACH</t>
+  </si>
+  <si>
+    <t>NOTE: CÂY NHỊ PHÂN TÌM KIẾM</t>
+  </si>
+  <si>
+    <t>HO</t>
+  </si>
+  <si>
+    <t>TEN</t>
+  </si>
+  <si>
+    <t>PHAI</t>
+  </si>
+  <si>
+    <t>NOTE: DANH SÁCH LIÊN KẾT ĐƠN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,8 +197,16 @@
       <charset val="163"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -151,8 +231,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -212,11 +322,114 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -248,6 +461,78 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -567,7 +852,7 @@
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -716,47 +1001,327 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A38A2D5-255B-4875-B229-79E683E1EA85}">
-  <dimension ref="B3:C7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B69E3B84-3787-4F17-BFF5-D2625967754B}">
+  <dimension ref="A3:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScale="76" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.5546875" customWidth="1"/>
+    <col min="2" max="2" width="12.21875" customWidth="1"/>
+    <col min="3" max="3" width="40" customWidth="1"/>
+    <col min="4" max="4" width="20.77734375" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" customWidth="1"/>
+    <col min="6" max="6" width="21.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="28" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
+      <c r="E4" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="20"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="28" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C5" t="s">
+      <c r="E5" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="20"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="28" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C6" t="s">
+      <c r="E6" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="20"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="28" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+      <c r="E7" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="20"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="20"/>
+      <c r="B9" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="29" t="s">
         <v>16</v>
       </c>
-    </row>
+      <c r="F9" s="22"/>
+      <c r="G9" s="23"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="20"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="24"/>
+      <c r="G10" s="25"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="20"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="24"/>
+      <c r="G11" s="25"/>
+    </row>
+    <row r="12" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="20"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="24"/>
+      <c r="G12" s="25"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="20"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="34" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="20"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="34" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="20"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="20"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="20"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="20"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="G18" s="34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="20"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19" s="34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="20"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="35"/>
+    </row>
+    <row r="21" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="20"/>
+      <c r="B21" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="35"/>
+      <c r="G21" s="35"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="20"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" s="35"/>
+      <c r="G22" s="35"/>
+    </row>
+    <row r="23" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="20"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="35"/>
+      <c r="G23" s="35"/>
+    </row>
+    <row r="24" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="20"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" s="35"/>
+      <c r="G24" s="35"/>
+    </row>
+    <row r="25" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E15:E19"/>
+    <mergeCell ref="F9:G12"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="C21:C24"/>
+    <mergeCell ref="A4:A24"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="B9:B19"/>
+    <mergeCell ref="C9:C19"/>
+    <mergeCell ref="D15:D19"/>
+    <mergeCell ref="D13:D14"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>